<commit_message>
Add per-voxel tissue classification and update classify func to also use std
</commit_message>
<xml_diff>
--- a/Results/IVIM_GTparamErrors_Detail_2025-07-10.xlsx
+++ b/Results/IVIM_GTparamErrors_Detail_2025-07-10.xlsx
@@ -635,17 +635,17 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>0.01199366041437366</v>
+        <v>0.01151337771989861</v>
       </c>
       <c r="H2" t="n">
-        <v>0.8723331689834595</v>
+        <v>0.9713624715805054</v>
       </c>
       <c r="I2" t="n">
-        <v>0.799121081829071</v>
+        <v>0.9740626215934753</v>
       </c>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="n">
-        <v>0.9547244906425476</v>
+        <v>1.232115983963013</v>
       </c>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="n">
@@ -655,10 +655,10 @@
         <v>0.001999999396502972</v>
       </c>
       <c r="O2" t="n">
-        <v>0.0003846059262286872</v>
+        <v>0.0003832288493867964</v>
       </c>
       <c r="P2" t="n">
-        <v>0.002780677285045385</v>
+        <v>0.003079316345974803</v>
       </c>
       <c r="Q2" t="n">
         <v>0.003000020515173674</v>
@@ -667,10 +667,10 @@
         <v>0.01999999396502972</v>
       </c>
       <c r="S2" t="n">
-        <v>0.004988208878785372</v>
+        <v>0.001205613720230758</v>
       </c>
       <c r="T2" t="n">
-        <v>0.02601191215217113</v>
+        <v>0.02743000164628029</v>
       </c>
       <c r="U2" t="inlineStr"/>
       <c r="V2" t="inlineStr"/>
@@ -683,17 +683,17 @@
         <v>0.6499997973442078</v>
       </c>
       <c r="AA2" t="n">
-        <v>0.04251236468553543</v>
+        <v>0.02987342700362206</v>
       </c>
       <c r="AB2" t="n">
-        <v>0.8034901022911072</v>
+        <v>0.9591321349143982</v>
       </c>
       <c r="AC2" t="inlineStr"/>
       <c r="AD2" t="inlineStr"/>
       <c r="AE2" t="inlineStr"/>
       <c r="AF2" t="inlineStr"/>
       <c r="AG2" t="n">
-        <v>0.8753929138183594</v>
+        <v>1.059180359045665</v>
       </c>
       <c r="AH2" t="inlineStr">
         <is>
@@ -731,17 +731,17 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>0.01270695592299711</v>
+        <v>0.01210435695255808</v>
       </c>
       <c r="H3" t="n">
-        <v>0.8033668398857117</v>
+        <v>0.8822528719902039</v>
       </c>
       <c r="I3" t="n">
-        <v>0.9306836724281311</v>
+        <v>0.9239464998245239</v>
       </c>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="n">
-        <v>1.138936758041382</v>
+        <v>1.133576393127441</v>
       </c>
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="n">
@@ -751,10 +751,10 @@
         <v>0.001999999396502972</v>
       </c>
       <c r="O3" t="n">
-        <v>0.0003764001885429025</v>
+        <v>0.0003655464679468423</v>
       </c>
       <c r="P3" t="n">
-        <v>0.002475346205756068</v>
+        <v>0.002732190303504467</v>
       </c>
       <c r="Q3" t="n">
         <v>0.003000020515173674</v>
@@ -763,10 +763,10 @@
         <v>0.01999999396502972</v>
       </c>
       <c r="S3" t="n">
-        <v>0.0005192756070755422</v>
+        <v>0.0005077528185211122</v>
       </c>
       <c r="T3" t="n">
-        <v>0.02437517605721951</v>
+        <v>0.02438162826001644</v>
       </c>
       <c r="U3" t="inlineStr"/>
       <c r="V3" t="inlineStr"/>
@@ -779,17 +779,17 @@
         <v>0.6499997973442078</v>
       </c>
       <c r="AA3" t="n">
-        <v>0.02710752002894878</v>
+        <v>0.02791030146181583</v>
       </c>
       <c r="AB3" t="n">
-        <v>0.8391681313514709</v>
+        <v>0.8385372757911682</v>
       </c>
       <c r="AC3" t="inlineStr"/>
       <c r="AD3" t="inlineStr"/>
       <c r="AE3" t="inlineStr"/>
       <c r="AF3" t="inlineStr"/>
       <c r="AG3" t="n">
-        <v>0.9576624234517416</v>
+        <v>0.979925254980723</v>
       </c>
       <c r="AH3" t="inlineStr">
         <is>
@@ -827,17 +827,17 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>0.02189195366215335</v>
+        <v>0.01668140465682543</v>
       </c>
       <c r="H4" t="n">
-        <v>0.1309442520141602</v>
+        <v>0.4516554176807404</v>
       </c>
       <c r="I4" t="n">
-        <v>0.3291864097118378</v>
+        <v>0.2733492851257324</v>
       </c>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="n">
-        <v>0.3547310531139374</v>
+        <v>0.4137914478778839</v>
       </c>
       <c r="L4" t="inlineStr"/>
       <c r="M4" t="n">
@@ -847,10 +847,10 @@
         <v>0.0007999998633749783</v>
       </c>
       <c r="O4" t="n">
-        <v>0.0006790816551074386</v>
+        <v>0.0007550443988293409</v>
       </c>
       <c r="P4" t="n">
-        <v>0.0008385346154682338</v>
+        <v>0.00113721948582679</v>
       </c>
       <c r="Q4" t="n">
         <v>0.004000117536634207</v>
@@ -859,10 +859,10 @@
         <v>0.01499997917562723</v>
       </c>
       <c r="S4" t="n">
-        <v>0.004063956439495087</v>
+        <v>0.005120145156979561</v>
       </c>
       <c r="T4" t="n">
-        <v>0.0167989544570446</v>
+        <v>0.01598424836993217</v>
       </c>
       <c r="U4" t="inlineStr"/>
       <c r="V4" t="inlineStr"/>
@@ -875,17 +875,17 @@
         <v>0.4999998211860657</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.2381947934627533</v>
+        <v>0.1917098462581635</v>
       </c>
       <c r="AB4" t="n">
-        <v>0.4362042546272278</v>
+        <v>0.4757309556007385</v>
       </c>
       <c r="AC4" t="inlineStr"/>
       <c r="AD4" t="inlineStr"/>
       <c r="AE4" t="inlineStr"/>
       <c r="AF4" t="inlineStr"/>
       <c r="AG4" t="n">
-        <v>0.2716205716133118</v>
+        <v>0.3795987168947856</v>
       </c>
       <c r="AH4" t="inlineStr">
         <is>
@@ -923,17 +923,17 @@
         </is>
       </c>
       <c r="G5" t="n">
-        <v>0.01167171238110136</v>
+        <v>0.01160455775164086</v>
       </c>
       <c r="H5" t="n">
-        <v>1.023898601531982</v>
+        <v>1.03947377204895</v>
       </c>
       <c r="I5" t="n">
-        <v>0.8674711585044861</v>
+        <v>0.8661603331565857</v>
       </c>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="n">
-        <v>0.9436420798301697</v>
+        <v>0.9199464917182922</v>
       </c>
       <c r="L5" t="inlineStr"/>
       <c r="M5" t="n">
@@ -943,10 +943,10 @@
         <v>0.0007999998633749783</v>
       </c>
       <c r="O5" t="n">
-        <v>0.0008563208975829184</v>
+        <v>0.0008607932250015438</v>
       </c>
       <c r="P5" t="n">
-        <v>0.002224985277280211</v>
+        <v>0.00236021657474339</v>
       </c>
       <c r="Q5" t="n">
         <v>0.004000117536634207</v>
@@ -955,10 +955,10 @@
         <v>0.01499997917562723</v>
       </c>
       <c r="S5" t="n">
-        <v>0.0006576697342097759</v>
+        <v>0.0006687275599688292</v>
       </c>
       <c r="T5" t="n">
-        <v>0.0242919959127903</v>
+        <v>0.0242635328322649</v>
       </c>
       <c r="U5" t="inlineStr"/>
       <c r="V5" t="inlineStr"/>
@@ -971,17 +971,17 @@
         <v>0.4999998211860657</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.02746119536459446</v>
+        <v>0.02682284638285637</v>
       </c>
       <c r="AB5" t="n">
-        <v>0.8383261561393738</v>
+        <v>0.8366816639900208</v>
       </c>
       <c r="AC5" t="inlineStr"/>
       <c r="AD5" t="inlineStr"/>
       <c r="AE5" t="inlineStr"/>
       <c r="AF5" t="inlineStr"/>
       <c r="AG5" t="n">
-        <v>0.9450039466222128</v>
+        <v>0.9418601989746094</v>
       </c>
       <c r="AH5" t="inlineStr">
         <is>
@@ -1019,17 +1019,17 @@
         </is>
       </c>
       <c r="G6" t="n">
-        <v>0.01292423384961169</v>
+        <v>0.0123147587745317</v>
       </c>
       <c r="H6" t="n">
-        <v>0.8721041083335876</v>
+        <v>0.9636647701263428</v>
       </c>
       <c r="I6" t="n">
-        <v>1.041630148887634</v>
+        <v>1.091870307922363</v>
       </c>
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="n">
-        <v>0.6979107260704041</v>
+        <v>0.7228075265884399</v>
       </c>
       <c r="L6" t="inlineStr"/>
       <c r="M6" t="n">
@@ -1039,10 +1039,10 @@
         <v>0.001399998553097248</v>
       </c>
       <c r="O6" t="n">
-        <v>0.00136992777697742</v>
+        <v>0.001362138194963336</v>
       </c>
       <c r="P6" t="n">
-        <v>0.002473544096574187</v>
+        <v>0.002728016814216971</v>
       </c>
       <c r="Q6" t="n">
         <v>0.004000012297183275</v>
@@ -1051,10 +1051,10 @@
         <v>0.01499999966472387</v>
       </c>
       <c r="S6" t="n">
-        <v>0.001757627236656845</v>
+        <v>0.0009068303625099361</v>
       </c>
       <c r="T6" t="n">
-        <v>0.02395269833505154</v>
+        <v>0.024044094607234</v>
       </c>
       <c r="U6" t="inlineStr"/>
       <c r="V6" t="inlineStr"/>
@@ -1067,17 +1067,17 @@
         <v>0.5999994874000549</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.03002902865409851</v>
+        <v>0.03323721885681152</v>
       </c>
       <c r="AB6" t="n">
-        <v>0.8264304995536804</v>
+        <v>0.8351407051086426</v>
       </c>
       <c r="AC6" t="inlineStr"/>
       <c r="AD6" t="inlineStr"/>
       <c r="AE6" t="inlineStr"/>
       <c r="AF6" t="inlineStr"/>
       <c r="AG6" t="n">
-        <v>0.8705483277638754</v>
+        <v>0.9261142015457153</v>
       </c>
       <c r="AH6" t="inlineStr">
         <is>
@@ -1115,17 +1115,17 @@
         </is>
       </c>
       <c r="G7" t="n">
-        <v>0.0231740599760936</v>
+        <v>0.01552071806581354</v>
       </c>
       <c r="H7" t="n">
-        <v>0.1996886432170868</v>
+        <v>0.6551063060760498</v>
       </c>
       <c r="I7" t="n">
-        <v>0.662761926651001</v>
+        <v>0.7163006067276001</v>
       </c>
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="n">
-        <v>0.4127302765846252</v>
+        <v>0.4502919912338257</v>
       </c>
       <c r="L7" t="inlineStr"/>
       <c r="M7" t="n">
@@ -1135,10 +1135,10 @@
         <v>0.001399998553097248</v>
       </c>
       <c r="O7" t="n">
-        <v>0.001179756596684456</v>
+        <v>0.001147853676229715</v>
       </c>
       <c r="P7" t="n">
-        <v>0.001500295358709991</v>
+        <v>0.002385001862421632</v>
       </c>
       <c r="Q7" t="n">
         <v>0.004000012297183275</v>
@@ -1147,10 +1147,10 @@
         <v>0.01499999966472387</v>
       </c>
       <c r="S7" t="n">
-        <v>0.001951959682628512</v>
+        <v>0.001609709113836288</v>
       </c>
       <c r="T7" t="n">
-        <v>0.01744435168802738</v>
+        <v>0.01772563718259335</v>
       </c>
       <c r="U7" t="inlineStr"/>
       <c r="V7" t="inlineStr"/>
@@ -1163,17 +1163,17 @@
         <v>0.5999994874000549</v>
       </c>
       <c r="AA7" t="n">
-        <v>0.2254485487937927</v>
+        <v>0.2233676910400391</v>
       </c>
       <c r="AB7" t="n">
-        <v>0.6776108741760254</v>
+        <v>0.6873108148574829</v>
       </c>
       <c r="AC7" t="inlineStr"/>
       <c r="AD7" t="inlineStr"/>
       <c r="AE7" t="inlineStr"/>
       <c r="AF7" t="inlineStr"/>
       <c r="AG7" t="n">
-        <v>0.4250602821509044</v>
+        <v>0.6072329680124918</v>
       </c>
       <c r="AH7" t="inlineStr">
         <is>
@@ -1211,22 +1211,22 @@
         </is>
       </c>
       <c r="G8" t="n">
-        <v>0.004924578154834483</v>
+        <v>0.004924585548700016</v>
       </c>
       <c r="H8" t="n">
-        <v>0.3551428914070129</v>
+        <v>0.3551428020000458</v>
       </c>
       <c r="I8" t="n">
-        <v>0.9733160734176636</v>
+        <v>0.973315417766571</v>
       </c>
       <c r="J8" t="n">
         <v>0.3624366223812103</v>
       </c>
       <c r="K8" t="n">
-        <v>0.3685720562934875</v>
+        <v>0.3685720264911652</v>
       </c>
       <c r="L8" t="n">
-        <v>0.4240774512290955</v>
+        <v>0.424077570438385</v>
       </c>
       <c r="M8" t="n">
         <v>0.0008000004454515874</v>
@@ -1235,7 +1235,7 @@
         <v>0.001799999736249447</v>
       </c>
       <c r="O8" t="n">
-        <v>0.0006675227778032422</v>
+        <v>0.0006675229524262249</v>
       </c>
       <c r="P8" t="n">
         <v>0.002064918866381049</v>
@@ -1247,7 +1247,7 @@
         <v>0.2399998605251312</v>
       </c>
       <c r="S8" t="n">
-        <v>0.005259193945676088</v>
+        <v>0.005259139463305473</v>
       </c>
       <c r="T8" t="n">
         <v>0.3023790717124939</v>
@@ -1271,10 +1271,10 @@
         <v>0.2399996966123581</v>
       </c>
       <c r="AA8" t="n">
-        <v>0.0747547447681427</v>
+        <v>0.07475495338439941</v>
       </c>
       <c r="AB8" t="n">
-        <v>0.2383793443441391</v>
+        <v>0.2383793741464615</v>
       </c>
       <c r="AC8" t="n">
         <v>0.16000035405159</v>
@@ -1283,13 +1283,13 @@
         <v>0.4799993634223938</v>
       </c>
       <c r="AE8" t="n">
-        <v>0.1163476854562759</v>
+        <v>0.1163476556539536</v>
       </c>
       <c r="AF8" t="n">
         <v>0.5529208183288574</v>
       </c>
       <c r="AG8" t="n">
-        <v>0.4967090487480164</v>
+        <v>0.496708869934082</v>
       </c>
       <c r="AH8" t="inlineStr">
         <is>
@@ -1327,22 +1327,22 @@
         </is>
       </c>
       <c r="G9" t="n">
-        <v>0.03538192117102206</v>
+        <v>0.02874025769672518</v>
       </c>
       <c r="H9" t="n">
-        <v>0.4502158761024475</v>
+        <v>0.2678773999214172</v>
       </c>
       <c r="I9" t="n">
-        <v>0.5487787127494812</v>
+        <v>0.5457256436347961</v>
       </c>
       <c r="J9" t="n">
-        <v>0.231552317738533</v>
+        <v>0.225668802857399</v>
       </c>
       <c r="K9" t="n">
-        <v>1.002182006835938</v>
+        <v>0.9990779161453247</v>
       </c>
       <c r="L9" t="n">
-        <v>0.7708754539489746</v>
+        <v>0.7727468609809875</v>
       </c>
       <c r="M9" t="n">
         <v>0.0008000004454515874</v>
@@ -1351,10 +1351,10 @@
         <v>0.001799999736249447</v>
       </c>
       <c r="O9" t="n">
-        <v>0.0006010314682498574</v>
+        <v>0.000720634707249701</v>
       </c>
       <c r="P9" t="n">
-        <v>0.0008067808812484145</v>
+        <v>0.00114066747482866</v>
       </c>
       <c r="Q9" t="n">
         <v>0.03200006484985352</v>
@@ -1363,10 +1363,10 @@
         <v>0.2399998605251312</v>
       </c>
       <c r="S9" t="n">
-        <v>0.09048549830913544</v>
+        <v>0.08453293144702911</v>
       </c>
       <c r="T9" t="n">
-        <v>0.09328349679708481</v>
+        <v>0.1011298894882202</v>
       </c>
       <c r="U9" t="n">
         <v>0.002200000686571002</v>
@@ -1375,10 +1375,10 @@
         <v>0.004799994174391031</v>
       </c>
       <c r="W9" t="n">
-        <v>0.002156795002520084</v>
+        <v>0.002126249019056559</v>
       </c>
       <c r="X9" t="n">
-        <v>0.003398883156478405</v>
+        <v>0.003451928496360779</v>
       </c>
       <c r="Y9" t="n">
         <v>0.08000010251998901</v>
@@ -1387,10 +1387,10 @@
         <v>0.2399996966123581</v>
       </c>
       <c r="AA9" t="n">
-        <v>0.005578216165304184</v>
+        <v>0.005271779838949442</v>
       </c>
       <c r="AB9" t="n">
-        <v>0.007340321317315102</v>
+        <v>0.007674264255911112</v>
       </c>
       <c r="AC9" t="n">
         <v>0.16000035405159</v>
@@ -1399,13 +1399,13 @@
         <v>0.4799993634223938</v>
       </c>
       <c r="AE9" t="n">
-        <v>0.05822053551673889</v>
+        <v>0.05569181591272354</v>
       </c>
       <c r="AF9" t="n">
-        <v>0.09419532120227814</v>
+        <v>0.09500941634178162</v>
       </c>
       <c r="AG9" t="n">
-        <v>0.6007208824157715</v>
+        <v>0.5622192621231079</v>
       </c>
       <c r="AH9" t="inlineStr">
         <is>
@@ -1443,22 +1443,22 @@
         </is>
       </c>
       <c r="G10" t="n">
-        <v>0.00864396468018999</v>
+        <v>0.008841533625893756</v>
       </c>
       <c r="H10" t="n">
-        <v>0.4640930891036987</v>
+        <v>0.4651162624359131</v>
       </c>
       <c r="I10" t="n">
-        <v>0.7139367461204529</v>
+        <v>0.7494789958000183</v>
       </c>
       <c r="J10" t="n">
-        <v>0.4889897108078003</v>
+        <v>0.4679813086986542</v>
       </c>
       <c r="K10" t="n">
-        <v>0.4320403933525085</v>
+        <v>0.3971155285835266</v>
       </c>
       <c r="L10" t="n">
-        <v>0.6069399118423462</v>
+        <v>0.5812245011329651</v>
       </c>
       <c r="M10" t="n">
         <v>0.0008000004454515874</v>
@@ -1467,10 +1467,10 @@
         <v>0.001799999736249447</v>
       </c>
       <c r="O10" t="n">
-        <v>0.0006960380123928189</v>
+        <v>0.0007019435288384557</v>
       </c>
       <c r="P10" t="n">
-        <v>0.002234057523310184</v>
+        <v>0.002226876560598612</v>
       </c>
       <c r="Q10" t="n">
         <v>0.03200006484985352</v>
@@ -1479,10 +1479,10 @@
         <v>0.2399998605251312</v>
       </c>
       <c r="S10" t="n">
-        <v>0.0128130316734314</v>
+        <v>0.01292955130338669</v>
       </c>
       <c r="T10" t="n">
-        <v>0.3053675591945648</v>
+        <v>0.2996516525745392</v>
       </c>
       <c r="U10" t="n">
         <v>0.002200000686571002</v>
@@ -1491,10 +1491,10 @@
         <v>0.004799994174391031</v>
       </c>
       <c r="W10" t="n">
-        <v>0.001093772007152438</v>
+        <v>0.00112334021832794</v>
       </c>
       <c r="X10" t="n">
-        <v>0.004721334669739008</v>
+        <v>0.004853658378124237</v>
       </c>
       <c r="Y10" t="n">
         <v>0.08000010251998901</v>
@@ -1503,10 +1503,10 @@
         <v>0.2399996966123581</v>
       </c>
       <c r="AA10" t="n">
-        <v>0.04530314356088638</v>
+        <v>0.05113017559051514</v>
       </c>
       <c r="AB10" t="n">
-        <v>0.2934457659721375</v>
+        <v>0.2702991664409637</v>
       </c>
       <c r="AC10" t="n">
         <v>0.16000035405159</v>
@@ -1515,13 +1515,13 @@
         <v>0.4799993634223938</v>
       </c>
       <c r="AE10" t="n">
-        <v>0.09004416316747665</v>
+        <v>0.09039118885993958</v>
       </c>
       <c r="AF10" t="n">
-        <v>0.6109588742256165</v>
+        <v>0.6086510419845581</v>
       </c>
       <c r="AG10" t="n">
-        <v>0.5411999821662903</v>
+        <v>0.5321832895278931</v>
       </c>
       <c r="AH10" t="inlineStr">
         <is>
@@ -1559,22 +1559,22 @@
         </is>
       </c>
       <c r="G11" t="n">
-        <v>0.005433878089681876</v>
+        <v>0.00543388015668324</v>
       </c>
       <c r="H11" t="n">
-        <v>0.371183842420578</v>
+        <v>0.3711841702461243</v>
       </c>
       <c r="I11" t="n">
-        <v>0.9824886918067932</v>
+        <v>0.9824885725975037</v>
       </c>
       <c r="J11" t="n">
-        <v>0.40048548579216</v>
+        <v>0.4004856050014496</v>
       </c>
       <c r="K11" t="n">
-        <v>0.4646075963973999</v>
+        <v>0.4646075367927551</v>
       </c>
       <c r="L11" t="n">
-        <v>0.538439929485321</v>
+        <v>0.5384392738342285</v>
       </c>
       <c r="M11" t="n">
         <v>0.0008000004454515874</v>
@@ -1583,10 +1583,10 @@
         <v>0.001799999736249447</v>
       </c>
       <c r="O11" t="n">
-        <v>0.0005774566670879722</v>
+        <v>0.0005774568999186158</v>
       </c>
       <c r="P11" t="n">
-        <v>0.002084414009004831</v>
+        <v>0.002084414241835475</v>
       </c>
       <c r="Q11" t="n">
         <v>0.03200006484985352</v>
@@ -1595,7 +1595,7 @@
         <v>0.2399998605251312</v>
       </c>
       <c r="S11" t="n">
-        <v>0.002839923603460193</v>
+        <v>0.002839930122718215</v>
       </c>
       <c r="T11" t="n">
         <v>0.3023839294910431</v>
@@ -1610,7 +1610,7 @@
         <v>0.001513349125161767</v>
       </c>
       <c r="X11" t="n">
-        <v>0.005421719048172235</v>
+        <v>0.005421718582510948</v>
       </c>
       <c r="Y11" t="n">
         <v>0.08000010251998901</v>
@@ -1619,10 +1619,10 @@
         <v>0.2399996966123581</v>
       </c>
       <c r="AA11" t="n">
-        <v>0.04786508902907372</v>
+        <v>0.04786508530378342</v>
       </c>
       <c r="AB11" t="n">
-        <v>0.1809943914413452</v>
+        <v>0.1809942871332169</v>
       </c>
       <c r="AC11" t="n">
         <v>0.16000035405159</v>
@@ -1631,13 +1631,13 @@
         <v>0.4799993634223938</v>
       </c>
       <c r="AE11" t="n">
-        <v>0.09099296480417252</v>
+        <v>0.09099282324314117</v>
       </c>
       <c r="AF11" t="n">
         <v>0.5718421936035156</v>
       </c>
       <c r="AG11" t="n">
-        <v>0.5514411330223083</v>
+        <v>0.5514410734176636</v>
       </c>
       <c r="AH11" t="inlineStr">
         <is>
@@ -1675,22 +1675,22 @@
         </is>
       </c>
       <c r="G12" t="n">
-        <v>0.006401019902301192</v>
+        <v>0.006840906843222927</v>
       </c>
       <c r="H12" t="n">
-        <v>0.243241623044014</v>
+        <v>0.2617772221565247</v>
       </c>
       <c r="I12" t="n">
-        <v>0.1154689118266106</v>
+        <v>0.1154575347900391</v>
       </c>
       <c r="J12" t="n">
-        <v>0.2177522331476212</v>
+        <v>0.211727112531662</v>
       </c>
       <c r="K12" t="n">
-        <v>0.1178162693977356</v>
+        <v>0.1203802824020386</v>
       </c>
       <c r="L12" t="n">
-        <v>0.2447931468486786</v>
+        <v>0.2355370372533798</v>
       </c>
       <c r="M12" t="n">
         <v>0.0005000001983717084</v>
@@ -1699,10 +1699,10 @@
         <v>0.0007399998139590025</v>
       </c>
       <c r="O12" t="n">
-        <v>0.0004355169367045164</v>
+        <v>0.000376757321646437</v>
       </c>
       <c r="P12" t="n">
-        <v>0.000635487143881619</v>
+        <v>0.0006864636670798063</v>
       </c>
       <c r="Q12" t="n">
         <v>0.07360001653432846</v>
@@ -1711,10 +1711,10 @@
         <v>0.1103999763727188</v>
       </c>
       <c r="S12" t="n">
-        <v>0.09147416055202484</v>
+        <v>0.09151735156774521</v>
       </c>
       <c r="T12" t="n">
-        <v>0.0928327888250351</v>
+        <v>0.09244311600923538</v>
       </c>
       <c r="U12" t="n">
         <v>0.002120011253282428</v>
@@ -1723,10 +1723,10 @@
         <v>0.003179997904226184</v>
       </c>
       <c r="W12" t="n">
-        <v>0.001960274763405323</v>
+        <v>0.001964043127372861</v>
       </c>
       <c r="X12" t="n">
-        <v>0.00249749212525785</v>
+        <v>0.002532760379835963</v>
       </c>
       <c r="Y12" t="n">
         <v>0.004800002556294203</v>
@@ -1735,10 +1735,10 @@
         <v>0.007199999876320362</v>
       </c>
       <c r="AA12" t="n">
-        <v>0.005733438767492771</v>
+        <v>0.005657235626131296</v>
       </c>
       <c r="AB12" t="n">
-        <v>0.006027959287166595</v>
+        <v>0.005966296419501305</v>
       </c>
       <c r="AC12" t="n">
         <v>0.05840004980564117</v>
@@ -1747,13 +1747,13 @@
         <v>0.08759989589452744</v>
       </c>
       <c r="AE12" t="n">
-        <v>0.05234883725643158</v>
+        <v>0.05299007892608643</v>
       </c>
       <c r="AF12" t="n">
-        <v>0.06826288253068924</v>
+        <v>0.067079097032547</v>
       </c>
       <c r="AG12" t="n">
-        <v>0.1878144294023514</v>
+        <v>0.1889758408069611</v>
       </c>
       <c r="AH12" t="inlineStr">
         <is>
@@ -1791,22 +1791,22 @@
         </is>
       </c>
       <c r="G13" t="n">
-        <v>0.003620247983229492</v>
+        <v>0.003620246360953677</v>
       </c>
       <c r="H13" t="n">
-        <v>0.1239967569708824</v>
+        <v>0.1239973306655884</v>
       </c>
       <c r="I13" t="n">
-        <v>0.9421275854110718</v>
+        <v>0.9421273469924927</v>
       </c>
       <c r="J13" t="n">
-        <v>0.6339676380157471</v>
+        <v>0.6339672207832336</v>
       </c>
       <c r="K13" t="n">
-        <v>19.04895401000977</v>
+        <v>19.04897117614746</v>
       </c>
       <c r="L13" t="n">
-        <v>0.4745123684406281</v>
+        <v>0.4745132923126221</v>
       </c>
       <c r="M13" t="n">
         <v>0.0005000001983717084</v>
@@ -1815,10 +1815,10 @@
         <v>0.0007399998139590025</v>
       </c>
       <c r="O13" t="n">
-        <v>0.0005437747458927333</v>
+        <v>0.0005437743384391069</v>
       </c>
       <c r="P13" t="n">
-        <v>0.0007107684505172074</v>
+        <v>0.0007107670535333455</v>
       </c>
       <c r="Q13" t="n">
         <v>0.07360001653432846</v>
@@ -1827,10 +1827,10 @@
         <v>0.1103999763727188</v>
       </c>
       <c r="S13" t="n">
-        <v>8.007788710528985e-05</v>
+        <v>8.007758151507005e-05</v>
       </c>
       <c r="T13" t="n">
-        <v>0.2819907963275909</v>
+        <v>0.2819909155368805</v>
       </c>
       <c r="U13" t="n">
         <v>0.002120011253282428</v>
@@ -1839,10 +1839,10 @@
         <v>0.003179997904226184</v>
       </c>
       <c r="W13" t="n">
-        <v>0.001493622548878193</v>
+        <v>0.001493622316047549</v>
       </c>
       <c r="X13" t="n">
-        <v>0.005511175375431776</v>
+        <v>0.005511174444109201</v>
       </c>
       <c r="Y13" t="n">
         <v>0.004800002556294203</v>
@@ -1851,10 +1851,10 @@
         <v>0.007199999876320362</v>
       </c>
       <c r="AA13" t="n">
-        <v>0.03666012734174728</v>
+        <v>0.03666011989116669</v>
       </c>
       <c r="AB13" t="n">
-        <v>0.2737361788749695</v>
+        <v>0.2737361490726471</v>
       </c>
       <c r="AC13" t="n">
         <v>0.05840004980564117</v>
@@ -1863,13 +1863,13 @@
         <v>0.08759989589452744</v>
       </c>
       <c r="AE13" t="n">
-        <v>0.07018546760082245</v>
+        <v>0.07018546015024185</v>
       </c>
       <c r="AF13" t="n">
-        <v>0.3689131140708923</v>
+        <v>0.3689137101173401</v>
       </c>
       <c r="AG13" t="n">
-        <v>4.244711875915527</v>
+        <v>4.244715690612793</v>
       </c>
       <c r="AH13" t="inlineStr">
         <is>
@@ -1907,22 +1907,22 @@
         </is>
       </c>
       <c r="G14" t="n">
-        <v>0.00439648871551969</v>
+        <v>0.004396437377464878</v>
       </c>
       <c r="H14" t="n">
-        <v>0.1618521213531494</v>
+        <v>0.1618513613939285</v>
       </c>
       <c r="I14" t="n">
-        <v>0.9670292735099792</v>
+        <v>0.967029333114624</v>
       </c>
       <c r="J14" t="n">
-        <v>0.8006477952003479</v>
+        <v>0.800649106502533</v>
       </c>
       <c r="K14" t="n">
-        <v>14.18457412719727</v>
+        <v>14.18455410003662</v>
       </c>
       <c r="L14" t="n">
-        <v>1.157567381858826</v>
+        <v>1.157567739486694</v>
       </c>
       <c r="M14" t="n">
         <v>0.0005000001983717084</v>
@@ -1931,10 +1931,10 @@
         <v>0.0007399998139590025</v>
       </c>
       <c r="O14" t="n">
-        <v>0.0005796937039121985</v>
+        <v>0.0005796921905130148</v>
       </c>
       <c r="P14" t="n">
-        <v>0.0008288143435493112</v>
+        <v>0.000828810385428369</v>
       </c>
       <c r="Q14" t="n">
         <v>0.07360001653432846</v>
@@ -1943,7 +1943,7 @@
         <v>0.1103999763727188</v>
       </c>
       <c r="S14" t="n">
-        <v>0.001505466760136187</v>
+        <v>0.001505465945228934</v>
       </c>
       <c r="T14" t="n">
         <v>0.005470860283821821</v>
@@ -1955,10 +1955,10 @@
         <v>0.003179997904226184</v>
       </c>
       <c r="W14" t="n">
-        <v>4.416443698573858e-05</v>
+        <v>4.416401498019695e-05</v>
       </c>
       <c r="X14" t="n">
-        <v>0.01429946813732386</v>
+        <v>0.01429929304867983</v>
       </c>
       <c r="Y14" t="n">
         <v>0.004800002556294203</v>
@@ -1967,10 +1967,10 @@
         <v>0.007199999876320362</v>
       </c>
       <c r="AA14" t="n">
-        <v>0.07334256917238235</v>
+        <v>0.07334248721599579</v>
       </c>
       <c r="AB14" t="n">
-        <v>0.219881683588028</v>
+        <v>0.2198814153671265</v>
       </c>
       <c r="AC14" t="n">
         <v>0.05840004980564117</v>
@@ -1979,13 +1979,13 @@
         <v>0.08759989589452744</v>
       </c>
       <c r="AE14" t="n">
-        <v>0.03753839433193207</v>
+        <v>0.03753843531012535</v>
       </c>
       <c r="AF14" t="n">
-        <v>0.273512214422226</v>
+        <v>0.2735121548175812</v>
       </c>
       <c r="AG14" t="n">
-        <v>3.454334259033203</v>
+        <v>3.454330444335938</v>
       </c>
       <c r="AH14" t="inlineStr">
         <is>
@@ -2023,22 +2023,22 @@
         </is>
       </c>
       <c r="G15" t="n">
-        <v>0.003485079042965387</v>
+        <v>0.003161861500497358</v>
       </c>
       <c r="H15" t="n">
-        <v>0.06057682633399963</v>
+        <v>0.08322694152593613</v>
       </c>
       <c r="I15" t="n">
-        <v>0.1154702231287956</v>
+        <v>0.1154726520180702</v>
       </c>
       <c r="J15" t="n">
-        <v>0.1251306384801865</v>
+        <v>0.1439897567033768</v>
       </c>
       <c r="K15" t="n">
-        <v>0.1168760061264038</v>
+        <v>0.1222028210759163</v>
       </c>
       <c r="L15" t="n">
-        <v>0.126507356762886</v>
+        <v>0.1568233072757721</v>
       </c>
       <c r="M15" t="n">
         <v>0.0005000001983717084</v>
@@ -2047,10 +2047,10 @@
         <v>0.0007399998139590025</v>
       </c>
       <c r="O15" t="n">
-        <v>0.0004606919828802347</v>
+        <v>0.000432666449341923</v>
       </c>
       <c r="P15" t="n">
-        <v>0.0007749552605673671</v>
+        <v>0.0008251482504419982</v>
       </c>
       <c r="Q15" t="n">
         <v>0.07360001653432846</v>
@@ -2059,10 +2059,10 @@
         <v>0.1103999763727188</v>
       </c>
       <c r="S15" t="n">
-        <v>0.0916338711977005</v>
+        <v>0.09048037230968475</v>
       </c>
       <c r="T15" t="n">
-        <v>0.09257222712039948</v>
+        <v>0.09348085522651672</v>
       </c>
       <c r="U15" t="n">
         <v>0.002120011253282428</v>
@@ -2071,10 +2071,10 @@
         <v>0.003179997904226184</v>
       </c>
       <c r="W15" t="n">
-        <v>0.002212139079347253</v>
+        <v>0.00221128948032856</v>
       </c>
       <c r="X15" t="n">
-        <v>0.002942531136795878</v>
+        <v>0.002686037216335535</v>
       </c>
       <c r="Y15" t="n">
         <v>0.004800002556294203</v>
@@ -2083,10 +2083,10 @@
         <v>0.007199999876320362</v>
       </c>
       <c r="AA15" t="n">
-        <v>0.005750861018896103</v>
+        <v>0.00554733956232667</v>
       </c>
       <c r="AB15" t="n">
-        <v>0.006061481777578592</v>
+        <v>0.006020572502166033</v>
       </c>
       <c r="AC15" t="n">
         <v>0.05840004980564117</v>
@@ -2095,13 +2095,13 @@
         <v>0.08759989589452744</v>
       </c>
       <c r="AE15" t="n">
-        <v>0.05956819653511047</v>
+        <v>0.0602380596101284</v>
       </c>
       <c r="AF15" t="n">
-        <v>0.08339962363243103</v>
+        <v>0.07229113578796387</v>
       </c>
       <c r="AG15" t="n">
-        <v>0.1089122071862221</v>
+        <v>0.1243430823087692</v>
       </c>
       <c r="AH15" t="inlineStr">
         <is>
@@ -2139,22 +2139,22 @@
         </is>
       </c>
       <c r="G16" t="n">
-        <v>0.00449762529486901</v>
+        <v>0.003189379255411273</v>
       </c>
       <c r="H16" t="n">
-        <v>0.1675280034542084</v>
+        <v>0.1653623431921005</v>
       </c>
       <c r="I16" t="n">
-        <v>0.2372841387987137</v>
+        <v>0.2279850989580154</v>
       </c>
       <c r="J16" t="n">
-        <v>0.1678812503814697</v>
+        <v>0.1385359913110733</v>
       </c>
       <c r="K16" t="n">
-        <v>0.2420213967561722</v>
+        <v>0.2553870975971222</v>
       </c>
       <c r="L16" t="n">
-        <v>0.552863597869873</v>
+        <v>0.6114568710327148</v>
       </c>
       <c r="M16" t="n">
         <v>0.000670000328682363</v>
@@ -2163,10 +2163,10 @@
         <v>0.001009999425150454</v>
       </c>
       <c r="O16" t="n">
-        <v>0.0005674847634509206</v>
+        <v>0.0005876513314433396</v>
       </c>
       <c r="P16" t="n">
-        <v>0.000786461285315454</v>
+        <v>0.001069844700396061</v>
       </c>
       <c r="Q16" t="n">
         <v>0.06080003827810287</v>
@@ -2175,10 +2175,10 @@
         <v>0.09119998663663864</v>
       </c>
       <c r="S16" t="n">
-        <v>0.09108956158161163</v>
+        <v>0.08672814071178436</v>
       </c>
       <c r="T16" t="n">
-        <v>0.09232544153928757</v>
+        <v>0.09479235857725143</v>
       </c>
       <c r="U16" t="n">
         <v>0.002190000377595425</v>
@@ -2187,10 +2187,10 @@
         <v>0.003289999673143029</v>
       </c>
       <c r="W16" t="n">
-        <v>0.002101170364767313</v>
+        <v>0.002150169806554914</v>
       </c>
       <c r="X16" t="n">
-        <v>0.003377896500751376</v>
+        <v>0.003264743834733963</v>
       </c>
       <c r="Y16" t="n">
         <v>0.00600000936537981</v>
@@ -2199,10 +2199,10 @@
         <v>0.008999999612569809</v>
       </c>
       <c r="AA16" t="n">
-        <v>0.005758829414844513</v>
+        <v>0.005412353668361902</v>
       </c>
       <c r="AB16" t="n">
-        <v>0.006127883680164814</v>
+        <v>0.006337391212582588</v>
       </c>
       <c r="AC16" t="n">
         <v>0.1400002837181091</v>
@@ -2211,13 +2211,13 @@
         <v>0.2099999785423279</v>
       </c>
       <c r="AE16" t="n">
-        <v>0.05354457348585129</v>
+        <v>0.05796690657734871</v>
       </c>
       <c r="AF16" t="n">
-        <v>0.09446658939123154</v>
+        <v>0.08729492127895355</v>
       </c>
       <c r="AG16" t="n">
-        <v>0.2735156714916229</v>
+        <v>0.279745489358902</v>
       </c>
       <c r="AH16" t="inlineStr">
         <is>
@@ -2255,22 +2255,22 @@
         </is>
       </c>
       <c r="G17" t="n">
-        <v>0.003549551623545023</v>
+        <v>0.003549562341576687</v>
       </c>
       <c r="H17" t="n">
-        <v>0.1991704255342484</v>
+        <v>0.1991702616214752</v>
       </c>
       <c r="I17" t="n">
-        <v>0.9398079514503479</v>
+        <v>0.9398078322410583</v>
       </c>
       <c r="J17" t="n">
-        <v>0.3803981244564056</v>
+        <v>0.380398690700531</v>
       </c>
       <c r="K17" t="n">
-        <v>8.917675018310547</v>
+        <v>8.917668342590332</v>
       </c>
       <c r="L17" t="n">
-        <v>0.3743875324726105</v>
+        <v>0.374387800693512</v>
       </c>
       <c r="M17" t="n">
         <v>0.000670000328682363</v>
@@ -2279,10 +2279,10 @@
         <v>0.001009999425150454</v>
       </c>
       <c r="O17" t="n">
-        <v>0.0005992413498461246</v>
+        <v>0.0005992414662614465</v>
       </c>
       <c r="P17" t="n">
-        <v>0.001207622000947595</v>
+        <v>0.001207623397931457</v>
       </c>
       <c r="Q17" t="n">
         <v>0.06080003827810287</v>
@@ -2291,10 +2291,10 @@
         <v>0.09119998663663864</v>
       </c>
       <c r="S17" t="n">
-        <v>0.0002410329761914909</v>
+        <v>0.0002410327433608472</v>
       </c>
       <c r="T17" t="n">
-        <v>0.1134523376822472</v>
+        <v>0.1134524047374725</v>
       </c>
       <c r="U17" t="n">
         <v>0.002190000377595425</v>
@@ -2303,10 +2303,10 @@
         <v>0.003289999673143029</v>
       </c>
       <c r="W17" t="n">
-        <v>0.001495237345807254</v>
+        <v>0.00149523769505322</v>
       </c>
       <c r="X17" t="n">
-        <v>0.005465185269713402</v>
+        <v>0.005465185735374689</v>
       </c>
       <c r="Y17" t="n">
         <v>0.00600000936537981</v>
@@ -2315,10 +2315,10 @@
         <v>0.008999999612569809</v>
       </c>
       <c r="AA17" t="n">
-        <v>0.04018185287714005</v>
+        <v>0.04018182307481766</v>
       </c>
       <c r="AB17" t="n">
-        <v>0.2249409407377243</v>
+        <v>0.2249408066272736</v>
       </c>
       <c r="AC17" t="n">
         <v>0.1400002837181091</v>
@@ -2327,13 +2327,13 @@
         <v>0.2099999785423279</v>
       </c>
       <c r="AE17" t="n">
-        <v>0.07801661640405655</v>
+        <v>0.07801663130521774</v>
       </c>
       <c r="AF17" t="n">
-        <v>0.4528487026691437</v>
+        <v>0.4528492987155914</v>
       </c>
       <c r="AG17" t="n">
-        <v>2.162287950515747</v>
+        <v>2.162286520004272</v>
       </c>
       <c r="AH17" t="inlineStr">
         <is>
@@ -2371,22 +2371,22 @@
         </is>
       </c>
       <c r="G18" t="n">
-        <v>0.003153433979408901</v>
+        <v>0.003188136343445302</v>
       </c>
       <c r="H18" t="n">
-        <v>0.1626405417919159</v>
+        <v>0.1688420623540878</v>
       </c>
       <c r="I18" t="n">
-        <v>0.1158158183097839</v>
+        <v>0.1155920252203941</v>
       </c>
       <c r="J18" t="n">
-        <v>0.1296434104442596</v>
+        <v>0.1444335728883743</v>
       </c>
       <c r="K18" t="n">
-        <v>0.1165240854024887</v>
+        <v>0.1179208979010582</v>
       </c>
       <c r="L18" t="n">
-        <v>0.1399244964122772</v>
+        <v>0.1422343552112579</v>
       </c>
       <c r="M18" t="n">
         <v>0.000670000328682363</v>
@@ -2395,10 +2395,10 @@
         <v>0.001009999425150454</v>
       </c>
       <c r="O18" t="n">
-        <v>0.0006084538763388991</v>
+        <v>0.0005989593337289989</v>
       </c>
       <c r="P18" t="n">
-        <v>0.001049871207214892</v>
+        <v>0.001110919751226902</v>
       </c>
       <c r="Q18" t="n">
         <v>0.06080003827810287</v>
@@ -2407,10 +2407,10 @@
         <v>0.09119998663663864</v>
       </c>
       <c r="S18" t="n">
-        <v>0.07463560253381729</v>
+        <v>0.07592024654150009</v>
       </c>
       <c r="T18" t="n">
-        <v>0.076475590467453</v>
+        <v>0.0761096403002739</v>
       </c>
       <c r="U18" t="n">
         <v>0.002190000377595425</v>
@@ -2419,10 +2419,10 @@
         <v>0.003289999673143029</v>
       </c>
       <c r="W18" t="n">
-        <v>0.002242899732664227</v>
+        <v>0.002183524891734123</v>
       </c>
       <c r="X18" t="n">
-        <v>0.003169055562466383</v>
+        <v>0.003030417487025261</v>
       </c>
       <c r="Y18" t="n">
         <v>0.00600000936537981</v>
@@ -2431,10 +2431,10 @@
         <v>0.008999999612569809</v>
       </c>
       <c r="AA18" t="n">
-        <v>0.007198409177362919</v>
+        <v>0.007160503882914782</v>
       </c>
       <c r="AB18" t="n">
-        <v>0.007695173844695091</v>
+        <v>0.007576503790915012</v>
       </c>
       <c r="AC18" t="n">
         <v>0.1400002837181091</v>
@@ -2443,13 +2443,13 @@
         <v>0.2099999785423279</v>
       </c>
       <c r="AE18" t="n">
-        <v>0.1379183381795883</v>
+        <v>0.139468714594841</v>
       </c>
       <c r="AF18" t="n">
-        <v>0.2034173011779785</v>
+        <v>0.1905046999454498</v>
       </c>
       <c r="AG18" t="n">
-        <v>0.1329096853733063</v>
+        <v>0.1378045827150345</v>
       </c>
       <c r="AH18" t="inlineStr">
         <is>
@@ -2487,22 +2487,22 @@
         </is>
       </c>
       <c r="G19" t="n">
-        <v>0.00501894867594864</v>
+        <v>0.005018963427494277</v>
       </c>
       <c r="H19" t="n">
-        <v>0.1962891519069672</v>
+        <v>0.1962890923023224</v>
       </c>
       <c r="I19" t="n">
-        <v>1.167323589324951</v>
+        <v>1.16732382774353</v>
       </c>
       <c r="J19" t="n">
-        <v>0.4129111766815186</v>
+        <v>0.412911593914032</v>
       </c>
       <c r="K19" t="n">
-        <v>11.03543758392334</v>
+        <v>11.03548717498779</v>
       </c>
       <c r="L19" t="n">
-        <v>0.3522663712501526</v>
+        <v>0.3522665798664093</v>
       </c>
       <c r="M19" t="n">
         <v>0.000670000328682363</v>
@@ -2511,10 +2511,10 @@
         <v>0.001009999425150454</v>
       </c>
       <c r="O19" t="n">
-        <v>0.000603956519626081</v>
+        <v>0.0006039564032107592</v>
       </c>
       <c r="P19" t="n">
-        <v>0.001385747687891126</v>
+        <v>0.001385747920721769</v>
       </c>
       <c r="Q19" t="n">
         <v>0.06080003827810287</v>
@@ -2523,7 +2523,7 @@
         <v>0.09119998663663864</v>
       </c>
       <c r="S19" t="n">
-        <v>0.0004830235557164997</v>
+        <v>0.0004830221878364682</v>
       </c>
       <c r="T19" t="n">
         <v>0.3015730679035187</v>
@@ -2535,7 +2535,7 @@
         <v>0.003289999673143029</v>
       </c>
       <c r="W19" t="n">
-        <v>0.001530965440906584</v>
+        <v>0.001530966139398515</v>
       </c>
       <c r="X19" t="n">
         <v>0.005484056659042835</v>
@@ -2547,10 +2547,10 @@
         <v>0.008999999612569809</v>
       </c>
       <c r="AA19" t="n">
-        <v>0.04189308360219002</v>
+        <v>0.04189307242631912</v>
       </c>
       <c r="AB19" t="n">
-        <v>0.2591703534126282</v>
+        <v>0.2591704428195953</v>
       </c>
       <c r="AC19" t="n">
         <v>0.1400002837181091</v>
@@ -2559,13 +2559,13 @@
         <v>0.2099999785423279</v>
       </c>
       <c r="AE19" t="n">
-        <v>0.07709982991218567</v>
+        <v>0.07709980010986328</v>
       </c>
       <c r="AF19" t="n">
-        <v>0.3773894906044006</v>
+        <v>0.3773894309997559</v>
       </c>
       <c r="AG19" t="n">
-        <v>2.632845401763916</v>
+        <v>2.632855653762817</v>
       </c>
       <c r="AH19" t="inlineStr">
         <is>

</xml_diff>